<commit_message>
file ready for all employees
</commit_message>
<xml_diff>
--- a/public/record/ToCustomer_7784.xlsx
+++ b/public/record/ToCustomer_7784.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>EC 2nd Floor Restrooms MW Sewer Repair (PR1224)</t>
+    <t>Underground Hydronic HHW Piiping</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>08/19/2022</t>
+    <t>08/23/2022</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>???</t>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -46,6 +46,9 @@
     <t>TASK ORDER NO.</t>
   </si>
   <si>
+    <t>CSU CPP-001.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">DOCUMENTED BY </t>
   </si>
   <si>
@@ -70,63 +73,6 @@
     <t>NO. OF WORKERS</t>
   </si>
   <si>
-    <t>A &amp; M Lath and Plastering Inc</t>
-  </si>
-  <si>
-    <t>TEST-HM</t>
-  </si>
-  <si>
-    <t>Women's Restroom - Install new wall Tiles</t>
-  </si>
-  <si>
-    <t>setsets</t>
-  </si>
-  <si>
-    <t>tset</t>
-  </si>
-  <si>
-    <t>Men's Restroom - Remove wall Tiles</t>
-  </si>
-  <si>
-    <t>etsetes</t>
-  </si>
-  <si>
-    <t>ts</t>
-  </si>
-  <si>
-    <t>A C Pros Inc</t>
-  </si>
-  <si>
-    <t>tsets</t>
-  </si>
-  <si>
-    <t>Women's Restroom - Remove and reinstall existing p</t>
-  </si>
-  <si>
-    <t>548 Group Inc.</t>
-  </si>
-  <si>
-    <t>tsetst</t>
-  </si>
-  <si>
-    <t>Women's Restroom - Install new Floor Tiles</t>
-  </si>
-  <si>
-    <t>A J Construction Specialties, Inc.</t>
-  </si>
-  <si>
-    <t>etset</t>
-  </si>
-  <si>
-    <t>stesetset</t>
-  </si>
-  <si>
-    <t>Women's Restroom - Remove wall Tiles</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -148,69 +94,7 @@
     <t>Result</t>
   </si>
   <si>
-    <t>testtestetset</t>
-  </si>
-  <si>
-    <t>setsetset</t>
-  </si>
-  <si>
-    <t>TEST 1</t>
-  </si>
-  <si>
-    <t>tsetsetstset</t>
-  </si>
-  <si>
-    <t>steset</t>
-  </si>
-  <si>
-    <t>setsetsets</t>
-  </si>
-  <si>
-    <t>setstsets</t>
-  </si>
-  <si>
-    <t>sets</t>
-  </si>
-  <si>
-    <t>erteetsets</t>
-  </si>
-  <si>
-    <t>terterte</t>
-  </si>
-  <si>
-    <t>testset</t>
-  </si>
-  <si>
-    <t>erttsetset</t>
-  </si>
-  <si>
-    <t>testsetst</t>
-  </si>
-  <si>
-    <t>testsetset</t>
-  </si>
-  <si>
-    <t>tsetst4</t>
-  </si>
-  <si>
-    <t>erterte</t>
-  </si>
-  <si>
-    <t>testsetsteset</t>
-  </si>
-  <si>
-    <t>testsetssetset</t>
-  </si>
-  <si>
-    <t>tesetsetset</t>
-  </si>
-  <si>
     <t>NOTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST ITTEST ITTEST ITTEST ITTEST ITTEST ITTEST ITTEST ITTEST IT
-TEST ITTEST ITTEST ITTEST ITTEST IT
-TEST ITTEST IT</t>
   </si>
 </sst>
 </file>
@@ -273,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -653,6 +537,17 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -696,34 +591,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -738,6 +605,34 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -768,6 +663,35 @@
       <top style="dashed">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -775,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -925,6 +849,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,11 +864,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -955,6 +885,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -964,10 +897,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1334,7 +1297,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="115"/>
   </sheetViews>
@@ -1389,7 +1352,7 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="16">
-        <v>6410</v>
+        <v>6485</v>
       </c>
       <c r="G3" s="17"/>
       <c r="I3" s="3"/>
@@ -1399,31 +1362,31 @@
         <v>8</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" s="21"/>
     </row>
     <row r="5" ht="19.5" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="29"/>
@@ -1432,10 +1395,10 @@
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="33"/>
       <c r="F6" s="34"/>
@@ -1443,432 +1406,223 @@
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="38">
-        <v>2</v>
-      </c>
-      <c r="D7" s="39">
-        <v>8</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>19</v>
-      </c>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="42">
-        <v>3</v>
-      </c>
-      <c r="D8" s="43">
-        <v>5</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>22</v>
-      </c>
+      <c r="A8" s="36"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="44"/>
       <c r="G8" s="44"/>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="42">
-        <v>5</v>
-      </c>
-      <c r="D9" s="43">
-        <v>5</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>19</v>
-      </c>
+      <c r="A9" s="36"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="44"/>
       <c r="G9" s="44"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="42">
-        <v>5</v>
-      </c>
-      <c r="D10" s="43">
-        <v>80</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>27</v>
-      </c>
+      <c r="A10" s="36"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="44"/>
       <c r="G10" s="44"/>
     </row>
     <row r="11" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="42">
-        <v>5</v>
-      </c>
-      <c r="D11" s="43">
-        <v>9</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>30</v>
-      </c>
+      <c r="A11" s="36"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
     </row>
     <row r="12" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="42">
-        <v>1</v>
-      </c>
-      <c r="D12" s="43">
-        <v>9</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>27</v>
-      </c>
+      <c r="A12" s="36"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="44"/>
       <c r="G12" s="44"/>
     </row>
     <row r="13" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="42">
-        <v>1</v>
-      </c>
-      <c r="D13" s="43">
-        <v>9</v>
-      </c>
-      <c r="E13" s="45" t="s">
-        <v>30</v>
-      </c>
+      <c r="A13" s="36"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="45"/>
       <c r="G13" s="45"/>
     </row>
     <row r="14" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="42">
-        <v>15</v>
-      </c>
-      <c r="D14" s="43">
-        <v>9</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="42">
-        <v>10</v>
-      </c>
-      <c r="D15" s="43">
+      <c r="A14" s="36"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+    </row>
+    <row r="15" ht="24.75" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="48">
+        <f>=SUM(C7:C14)</f>
+      </c>
+      <c r="D15" s="48">
+        <f>=SUM(D7:D14)</f>
+      </c>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+    </row>
+    <row r="16" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="56"/>
+      <c r="E17" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="58"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" ht="18" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="66"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="44"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-    </row>
-    <row r="16" ht="24.75" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48">
-        <f>=SUM(C7:C15)</f>
-      </c>
-      <c r="D16" s="48">
-        <f>=SUM(D7:D15)</f>
-      </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-    </row>
-    <row r="17" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="53"/>
-      <c r="G18" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="58"/>
-      <c r="G19" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="60"/>
-      <c r="G22" s="61" t="s">
-        <v>32</v>
-      </c>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="72"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61" t="s">
-        <v>53</v>
-      </c>
+      <c r="A23" s="73"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="75"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="60"/>
-      <c r="G24" s="61" t="s">
-        <v>57</v>
-      </c>
+      <c r="A24" s="73"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="75"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="63"/>
-      <c r="G25" s="44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="66"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" ht="18" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
+      <c r="A25" s="76"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="78"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="79"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="80"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="79"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="79"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="80"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="67"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="66"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="66"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="67"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="66"/>
+      <c r="A31" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -1894,18 +1648,18 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="E15:G15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:G30"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:G25"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.46" right="0.32" top="0.58" bottom="0.45" header="0.57" footer="0.3"/>

</xml_diff>

<commit_message>
number bug when exporting excel
</commit_message>
<xml_diff>
--- a/public/record/ToCustomer_7784.xlsx
+++ b/public/record/ToCustomer_7784.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -73,12 +73,15 @@
     <t>NO. OF WORKERS</t>
   </si>
   <si>
+    <t>Northcon Inc</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>No on-site work</t>
-  </si>
-  <si>
     <t>INSPECTIONS</t>
   </si>
   <si>
@@ -98,9 +101,6 @@
   </si>
   <si>
     <t>NOTE</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -1412,11 +1412,21 @@
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
+      <c r="A7" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="38">
+        <v>4</v>
+      </c>
+      <c r="D7" s="39">
+        <v>0</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
@@ -1485,7 +1495,7 @@
     </row>
     <row r="15" ht="24.75" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="48">
@@ -1494,15 +1504,13 @@
       <c r="D15" s="48">
         <f>=SUM(D7:D14)</f>
       </c>
-      <c r="E15" s="49" t="s">
-        <v>19</v>
-      </c>
+      <c r="E15" s="49"/>
       <c r="F15" s="49"/>
       <c r="G15" s="49"/>
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
@@ -1514,21 +1522,21 @@
     </row>
     <row r="17" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="55" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" s="56"/>
       <c r="G17" s="57" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1563,7 +1571,7 @@
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" s="69"/>
       <c r="C21" s="69"/>
@@ -1575,7 +1583,7 @@
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B22" s="71"/>
       <c r="C22" s="71"/>

</xml_diff>

<commit_message>
db Exbon -> Hammer
</commit_message>
<xml_diff>
--- a/public/record/ToCustomer_7784.xlsx
+++ b/public/record/ToCustomer_7784.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,19 +25,19 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Desert HS Modernization</t>
+    <t>Repair HVAC Interior B10210</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>08/31/2022</t>
+    <t>08/22/2022</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>5976</t>
+    <t>RKMF 17-0133</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -46,7 +46,7 @@
     <t>TASK ORDER NO.</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>FA486118FA140</t>
   </si>
   <si>
     <t xml:space="preserve">DOCUMENTED BY </t>
@@ -73,12 +73,18 @@
     <t>NO. OF WORKERS</t>
   </si>
   <si>
+    <t>548 Group Inc.</t>
+  </si>
+  <si>
+    <t>Bldg 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Abatement</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>No on-site work</t>
-  </si>
-  <si>
     <t>INSPECTIONS</t>
   </si>
   <si>
@@ -97,10 +103,22 @@
     <t>Result</t>
   </si>
   <si>
+    <t>Inpsector A</t>
+  </si>
+  <si>
+    <t>LAISD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough Electrical </t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>NOTE</t>
   </si>
   <si>
-    <t/>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -1357,8 +1375,8 @@
         <v>7</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="16" t="s">
-        <v>6</v>
+      <c r="F3" s="16">
+        <v>5733</v>
       </c>
       <c r="G3" s="17"/>
       <c r="I3" s="3"/>
@@ -1412,11 +1430,21 @@
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
+      <c r="A7" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="38">
+        <v>1</v>
+      </c>
+      <c r="D7" s="39">
+        <v>1</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>20</v>
+      </c>
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
@@ -1485,7 +1513,7 @@
     </row>
     <row r="15" ht="24.75" customHeight="1" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="48">
@@ -1494,15 +1522,13 @@
       <c r="D15" s="48">
         <f>=SUM(D7:D14)</f>
       </c>
-      <c r="E15" s="49" t="s">
-        <v>19</v>
-      </c>
+      <c r="E15" s="49"/>
       <c r="F15" s="49"/>
       <c r="G15" s="49"/>
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
@@ -1514,32 +1540,42 @@
     </row>
     <row r="17" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="55" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F17" s="56"/>
       <c r="G17" s="57" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
+      <c r="A18" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>19</v>
+      </c>
       <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
+      <c r="E18" s="62" t="s">
+        <v>30</v>
+      </c>
       <c r="F18" s="63"/>
-      <c r="G18" s="64"/>
+      <c r="G18" s="64" t="s">
+        <v>31</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1563,7 +1599,7 @@
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B21" s="69"/>
       <c r="C21" s="69"/>
@@ -1575,7 +1611,7 @@
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B22" s="71"/>
       <c r="C22" s="71"/>

</xml_diff>